<commit_message>
membuat halaman juri tanding
</commit_message>
<xml_diff>
--- a/public/assets/template/gelanggang-template.xlsx
+++ b/public/assets/template/gelanggang-template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ndejo\Documents\GitHub\simaps-ukasya\public\assets\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0EC116E-6F02-472A-B8AC-56E4499FD311}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D50C9DA-0ACC-4BDA-B406-76AFB150B5F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{51F6D04B-38A7-4907-901E-8D2AF0D93E74}"/>
+    <workbookView xWindow="2205" yWindow="2205" windowWidth="15375" windowHeight="7875" xr2:uid="{51F6D04B-38A7-4907-901E-8D2AF0D93E74}"/>
   </bookViews>
   <sheets>
     <sheet name="Lembar1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
   <si>
     <t>Nama</t>
   </si>
@@ -45,6 +45,9 @@
     <t>Waktu</t>
   </si>
   <si>
+    <t>Audio</t>
+  </si>
+  <si>
     <t>Jenis</t>
   </si>
   <si>
@@ -58,6 +61,9 @@
   </si>
   <si>
     <t>Arena D</t>
+  </si>
+  <si>
+    <t>audio.mp3</t>
   </si>
   <si>
     <t>Tanding</t>
@@ -145,7 +151,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -488,50 +494,65 @@
       <c r="C1" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="D1" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="E1" s="3"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" s="1">
         <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" s="1">
         <v>3</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B4" s="1">
         <v>3</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>9</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B5" s="1">
         <v>3</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>